<commit_message>
Gestion des camp et registre de présence
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_registrepresence.xlsx
+++ b/fichiers/conf/modele_registrepresence.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717031B-26CE-43FF-9A95-230685D23D1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D6406D-E85B-48CF-A2F9-471B19BD5354}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1185" windowWidth="22905" windowHeight="13815" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
+    <workbookView xWindow="945" yWindow="720" windowWidth="26610" windowHeight="14445" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
   </bookViews>
   <sheets>
-    <sheet name="Activités" sheetId="1" r:id="rId1"/>
-    <sheet name="Activités mois" sheetId="3" r:id="rId2"/>
-    <sheet name="CEC" sheetId="2" r:id="rId3"/>
+    <sheet name="Activités par unité" sheetId="4" r:id="rId1"/>
+    <sheet name="Activités par unité et type" sheetId="1" r:id="rId2"/>
+    <sheet name="Activités mois" sheetId="3" r:id="rId3"/>
+    <sheet name="CEC" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Activités!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Activités mois'!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CEC!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Activités mois'!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Activités par unité'!$A$1:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Activités par unité et type'!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CEC!$A$1:$E$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
   </si>
@@ -76,19 +78,73 @@
     <t>${result.object.unitecourt}</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${activites}" aggs="Sum(heure)" valuesVar="results" groupBy="unite;type"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.groupe}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites}" aggs="Sum(heure)" valuesVar="results" groupBy="unite;moisactivite"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(1)"&gt;${result.object.groupe}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites}" aggs="Sum(heurechef)" valuesVar="results" groupBy="unite;type;nom"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(2)"&gt;${result.object.groupe}</t>
+    <t>&lt;jt:agg items="${activites_heures}" aggs="Sum(heure)" valuesVar="results" groupBy="unite;type"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.groupe}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_heures}" aggs="Sum(heure)" valuesVar="results" groupBy="unite;moisactivite"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(1)"&gt;${result.object.groupe}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_heures}" aggs="Sum(heurechef)" valuesVar="results" groupBy="unite;type;nom"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(2)"&gt;${result.object.groupe}</t>
+  </si>
+  <si>
+    <t>${activite.type}</t>
+  </si>
+  <si>
+    <t>&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Début</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>${activite.debut}</t>
+  </si>
+  <si>
+    <t>${activite.fin}</t>
+  </si>
+  <si>
+    <t>Remplissage</t>
+  </si>
+  <si>
+    <t>${activite.remplissage}</t>
+  </si>
+  <si>
+    <t>Présence Chefs</t>
+  </si>
+  <si>
+    <t>Présence Jeunes</t>
+  </si>
+  <si>
+    <t>${activite.presencechefs}</t>
+  </si>
+  <si>
+    <t>${activite.presencejeunes}</t>
+  </si>
+  <si>
+    <t>Présence Unité</t>
+  </si>
+  <si>
+    <t>$[G2+H2]</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${activites}" var="activite" orderBy="unite;debutnum"&gt;${activite.unite}</t>
+  </si>
+  <si>
+    <t>${activite.description}</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dddd\ dd/mm/yyyy\ hh:mm"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,11 +228,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -516,10 +584,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EBBEE7-15CD-4D5F-8A3D-CC65F98B5CBA}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I2" xr:uid="{51966C8B-6EEE-48DA-8AE4-BBFE01F1C6F9}"/>
+  <conditionalFormatting sqref="M2">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67877FCE-0AFF-4AEB-B17A-D7414C418278}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -573,11 +735,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFA6324-0B25-4F78-A5F1-6BF17C24617F}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -632,11 +796,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863F9A69-0B6D-44B1-8E43-463423A6A72E}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
reorgnisation du code pour la gestion du registre de présence
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_registrepresence.xlsx
+++ b/fichiers/conf/modele_registrepresence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AD9224-A24F-4777-8E33-8AF424F1D7CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9682AC3-7E79-411E-8FFA-4110AAF81E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="747" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
+    <workbookView xWindow="645" yWindow="900" windowWidth="25425" windowHeight="14160" tabRatio="747" activeTab="1" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="8" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Activités mois" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Activités chefs (détails)'!$A$1:$H$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Activités mois'!$A$1:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Activités par unité'!$A$1:$M$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Activités par unité et type'!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Activités chefs (détails)'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Activités mois'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Activités par unité'!$A$1:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Activités par unité et type'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Groupe</t>
-  </si>
-  <si>
-    <t>${result.object.unitecourt}</t>
-  </si>
-  <si>
     <t>${activite.type}</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Présence Unité</t>
   </si>
   <si>
-    <t>&lt;jt:forEach items="${activites}" var="activite" orderBy="unite;debutnum"&gt;${activite.unite}</t>
-  </si>
-  <si>
     <t>${activite.description}</t>
   </si>
   <si>
@@ -138,12 +129,6 @@
     <t>$[H2+I2]</t>
   </si>
   <si>
-    <t>Total groupe</t>
-  </si>
-  <si>
-    <t>Total par unité</t>
-  </si>
-  <si>
     <t>Durée (f)</t>
   </si>
   <si>
@@ -153,9 +138,6 @@
     <t>${activite.dureereel}</t>
   </si>
   <si>
-    <t>${activite.unite}</t>
-  </si>
-  <si>
     <t>${activite.nom}</t>
   </si>
   <si>
@@ -165,15 +147,6 @@
     <t>Nom</t>
   </si>
   <si>
-    <t>&lt;jt:forEach items="${activites_personnes}" var="activite" orderBy="unite;moisactivite" where="${activite.chef}"&gt;${activite.groupe}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite;type"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.groupe}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite;moisactivite"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(1)"&gt;${result.object.groupe}</t>
-  </si>
-  <si>
     <t>Nombre d'heures (r)</t>
   </si>
   <si>
@@ -183,12 +156,6 @@
     <t>${result.getAggregateValue(aggs[1])}</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.groupe}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite}</t>
-  </si>
-  <si>
     <t>Réel</t>
   </si>
   <si>
@@ -199,6 +166,48 @@
   </si>
   <si>
     <t>${activite.dureeforfaitairetotal}</t>
+  </si>
+  <si>
+    <t>Total structure</t>
+  </si>
+  <si>
+    <t>Total par sous-structure</t>
+  </si>
+  <si>
+    <t>Code Groupe</t>
+  </si>
+  <si>
+    <t>Code Structure</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${activites}" var="activite" orderBy="unite;debutnum"&gt;${activite.unite.codegroupe}</t>
+  </si>
+  <si>
+    <t>${activite.unite.codestructure}</t>
+  </si>
+  <si>
+    <t>${activite.unite.nom}</t>
+  </si>
+  <si>
+    <t>${result.object.unite.codestructure}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.nom}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.nom}</t>
+  </si>
+  <si>
+    <t>${result.object.unite.nom}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${activites_personnes}" var="activite" orderBy="unite;moisactivite" where="${activite.chef}"&gt;${activite.unite.groupe.code}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite;type"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.groupe.code}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite;moisactivite"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(1)"&gt;${result.object.unite.groupe.code}</t>
   </si>
 </sst>
 </file>
@@ -287,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,6 +319,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -689,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F6563-5187-4E25-A5A7-AB42223A1E83}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -700,24 +721,24 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -729,18 +750,18 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -759,121 +780,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EBBEE7-15CD-4D5F-8A3D-CC65F98B5CBA}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="G2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="M2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>10</v>
+      <c r="S2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M2" xr:uid="{09DCEFCB-17BE-4379-80B7-24E27D346FFA}"/>
-  <conditionalFormatting sqref="Q2">
+  <autoFilter ref="A1:O2" xr:uid="{1B94AA9D-E07C-42F5-96DC-6669C93F9B51}"/>
+  <conditionalFormatting sqref="S2">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H2048">
+  <conditionalFormatting sqref="J2:J2048">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -885,81 +919,85 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84716716-4801-4E0D-BBE9-352AF3EF6509}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="52.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="86.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
+      <c r="D1" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H2" xr:uid="{85E04011-F81B-4AAC-AA6E-E793D4B8E76D}"/>
-  <conditionalFormatting sqref="L2">
+  <autoFilter ref="A1:I1" xr:uid="{7B1C69B3-1BD0-46CA-B4D0-848488C3E47B}"/>
+  <conditionalFormatting sqref="M2">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -971,7 +1009,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67877FCE-0AFF-4AEB-B17A-D7414C418278}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -979,54 +1017,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.85546875" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="82.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2" xr:uid="{77D660DA-B143-40D2-A584-919C350B5D83}"/>
-  <conditionalFormatting sqref="L2">
+  <autoFilter ref="A1:F1" xr:uid="{2F16A6E1-160C-4FF3-A4DB-956F6B7BC913}"/>
+  <conditionalFormatting sqref="M2">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1037,60 +1081,68 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFA6324-0B25-4F78-A5F1-6BF17C24617F}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="85.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2" xr:uid="{4AB464EF-2468-4707-983A-4C1C7EDEFF83}"/>
-  <conditionalFormatting sqref="L2">
+  <autoFilter ref="A1:F1" xr:uid="{A689D2B1-AAF8-4676-B8F1-8DAA8385EBE6}"/>
+  <conditionalFormatting sqref="M2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Ajout des temps "jeunes" #35
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_registrepresence.xlsx
+++ b/fichiers/conf/modele_registrepresence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3211ECC1-064F-4503-BFAE-6C288617FB08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22AA2E-B27A-4A4B-A5EB-0F0B8CA8EE05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" tabRatio="747" activeTab="1" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="747" activeTab="1" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="10" r:id="rId1"/>
@@ -24,9 +24,9 @@
     <sheet name="Général" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Activités mois'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Activités par unité'!$A$1:$O$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Activités par unité et type'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Activités mois'!$A$2:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Activités par unité'!$A$2:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Activités par unité et type'!$A$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Bénévolat encadrement (CEC)'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
   <si>
     <t>&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
   </si>
@@ -196,24 +196,12 @@
     <t>${result.object.unite.codestructure}</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.nom}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.nom}</t>
-  </si>
-  <si>
     <t>${result.object.unite.nom}</t>
   </si>
   <si>
     <t>&lt;jt:forEach items="${activites_personnes}" var="activite" orderBy="unite;moisactivite" where="${activite.chef}"&gt;${activite.unite.groupe.code}</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite;type"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.groupe.code}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureeforfaitaire)" valuesVar="results" groupBy="unite;moisactivite"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(1)"&gt;${result.object.unite.groupe.code}</t>
-  </si>
-  <si>
     <t>Groupe</t>
   </si>
   <si>
@@ -224,6 +212,42 @@
   </si>
   <si>
     <t>${global.marins}</t>
+  </si>
+  <si>
+    <t>Réel (jeunes)</t>
+  </si>
+  <si>
+    <t>Forfait (jeunes)</t>
+  </si>
+  <si>
+    <t>${result.getAggregateValue(aggs[2])}</t>
+  </si>
+  <si>
+    <t>${result.getAggregateValue(aggs[3])}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureereeljeune);Sum(dureeforfaitaire);Sum(dureeforfaitairejeune)" groupBy="unite" valuesVar="results"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.nom}</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Jeunes</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureereeljeune);Sum(dureeforfaitaire);Sum(dureeforfaitairejeune)" valuesVar="results" groupBy="unite;type"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${result.object.unite.groupe.code}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureereeljeune);Sum(dureeforfaitaire);Sum(dureeforfaitairejeune)" valuesVar="results" groupBy="unite;moisactivite"&gt;&lt;jt:forEach items="${results}" var="result" orderBy="getPropertyValue(1)"&gt;${result.object.unite.groupe.code}</t>
+  </si>
+  <si>
+    <t>${activite.dureereeltotaljeune}</t>
+  </si>
+  <si>
+    <t>${activite.dureeforfaitairetotaljeune}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${activites_personnes}" aggs="Sum(dureereel);Sum(dureereeljeune);Sum(dureeforfaitaire);Sum(dureeforfaitairejeune)" valuesVar="results"&gt;&lt;jt:forEach items="${results}" var="result"&gt;${global.groupe}</t>
   </si>
 </sst>
 </file>
@@ -284,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -307,12 +331,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,13 +431,31 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
         <color theme="0"/>
@@ -394,6 +493,16 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -734,7 +843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -749,14 +858,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
+    <col min="1" max="1" width="67.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -764,12 +875,18 @@
         <v>37</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E1" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -777,22 +894,29 @@
       <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -800,13 +924,24 @@
       <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D5 R3 D2">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="R3 F2">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -824,7 +959,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -835,135 +970,163 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" customWidth="1"/>
-    <col min="3" max="3" width="59.7265625" customWidth="1"/>
-    <col min="4" max="4" width="59.26953125" customWidth="1"/>
-    <col min="5" max="5" width="29.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.90625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.36328125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="17.85546875" style="3" customWidth="1"/>
+    <col min="9" max="10" width="13" style="3" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12" style="3" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="G2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O2" xr:uid="{1B94AA9D-E07C-42F5-96DC-6669C93F9B51}"/>
-  <conditionalFormatting sqref="S2">
+  <autoFilter ref="A2:U2" xr:uid="{59F8BA04-5672-401D-B931-828BC8AB731F}"/>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="U3">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J2048">
+  <conditionalFormatting sqref="L3:L2049">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -980,21 +1143,23 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="86.453125" customWidth="1"/>
-    <col min="4" max="4" width="40.54296875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="86.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="12" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="52.81640625" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>43</v>
       </c>
@@ -1023,9 +1188,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -1072,67 +1237,93 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="82.453125" customWidth="1"/>
-    <col min="4" max="4" width="31.54296875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" customWidth="1"/>
-    <col min="13" max="13" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="82.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{2F16A6E1-160C-4FF3-A4DB-956F6B7BC913}"/>
-  <conditionalFormatting sqref="M2">
+  <autoFilter ref="A2:D2" xr:uid="{262A407E-25D5-4174-9F66-93AF4D7F5522}"/>
+  <mergeCells count="2">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="O3">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1146,67 +1337,93 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="85.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="19.90625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" customWidth="1"/>
-    <col min="13" max="13" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" style="19" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="3" customWidth="1"/>
+    <col min="6" max="8" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{A689D2B1-AAF8-4676-B8F1-8DAA8385EBE6}"/>
-  <conditionalFormatting sqref="M2">
+  <autoFilter ref="A2:D2" xr:uid="{122F8AB8-D872-4D55-9714-F54A24AD6CE3}"/>
+  <mergeCells count="2">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1222,26 +1439,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Analyse du registre de présence en année civile #36
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_registrepresence.xlsx
+++ b/fichiers/conf/modele_registrepresence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22AA2E-B27A-4A4B-A5EB-0F0B8CA8EE05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A1E270-776D-4831-94C3-F7A2A8EA499C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="747" activeTab="1" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
+    <workbookView xWindow="780" yWindow="405" windowWidth="25665" windowHeight="14580" tabRatio="747" activeTab="1" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="10" r:id="rId1"/>
@@ -441,14 +441,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1260,7 +1260,7 @@
       <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:15" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1339,7 +1339,9 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1356,11 +1358,11 @@
       <c r="E1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">

</xml_diff>